<commit_message>
Fixed TC course's schedule
</commit_message>
<xml_diff>
--- a/SecondSemester'sSchedule(1402-03).xlsx
+++ b/SecondSemester'sSchedule(1402-03).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AcademicMaterial\UniversityAffairs\Management\Plans\برنامه نیمسال دوم03-1402\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAMED FAHIMI\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9CD7DC-7182-49CD-9746-6F9A1F920A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0427D8F8-7DB3-4E46-8A5D-9C06AC741BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17323706-087C-48D1-97C3-2A4984637200}"/>
   </bookViews>
@@ -179,31 +179,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">برنامه سازی پیشرفته (تئوری-مهندس شریعتی)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t>نظریه محاسبه (دکتر خیرخواه)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>مبانی احتمال</t>
     </r>
     <r>
@@ -894,6 +869,10 @@
       </rPr>
       <t>´</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">برنامه سازی پیشرفته (تئوری-مهندس شریعتی)
+</t>
   </si>
 </sst>
 </file>
@@ -1140,28 +1119,52 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1170,49 +1173,25 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1542,7 +1521,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1586,33 +1565,33 @@
       <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="27"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="150.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="28"/>
+      <c r="I2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="21"/>
+      <c r="J2" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="1:11" ht="110.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -1621,38 +1600,38 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+        <v>36</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23" t="s">
+      <c r="A4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="28"/>
+      <c r="I4" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -1669,39 +1648,39 @@
         <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="24"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+        <v>39</v>
+      </c>
+      <c r="I5" s="32"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" ht="190.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="28" t="s">
+      <c r="A6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="29"/>
-      <c r="I6" s="24" t="s">
+      <c r="H6" s="34"/>
+      <c r="I6" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" ht="139.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="10"/>
@@ -1709,38 +1688,38 @@
         <v>17</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="15" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="35"/>
-      <c r="I8" s="24" t="s">
+      <c r="F8" s="20"/>
+      <c r="G8" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="22"/>
+      <c r="I8" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" ht="145.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="10" t="s">
@@ -1750,10 +1729,10 @@
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>15</v>
@@ -1761,36 +1740,36 @@
       <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="35"/>
-      <c r="I10" s="24" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1801,15 +1780,27 @@
         <v>19</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
+        <v>42</v>
+      </c>
+      <c r="I11" s="32"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="G2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J2:K11"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
@@ -1825,18 +1816,6 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J2:K11"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E2:F3"/>
-    <mergeCell ref="G2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="38" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Missing slot for DM added
</commit_message>
<xml_diff>
--- a/SecondSemester'sSchedule(1402-03).xlsx
+++ b/SecondSemester'sSchedule(1402-03).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniversityAffairs\Management\Schedules\برنامه نیمسال دوم03-1402\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478D0441-124D-486D-AEFE-97E085F99899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A05FA5B-0BEE-4AAA-835B-307B9A485424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17323706-087C-48D1-97C3-2A4984637200}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t xml:space="preserve">شنبه
 </t>
@@ -732,22 +732,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">
-آز سیستم عامل (مهندس مهندس شاه منصوری)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t>ریاضی عمومی 2 (دکتر اعتبار)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="18"/>
         <color rgb="FFFF0000"/>
@@ -877,6 +861,26 @@
   <si>
     <t xml:space="preserve">برنامه سازی پیشرفته (تئوری-مهندس شریعتی)
 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+آز سیستم عامل (مهندس شاه منصوری)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>ریاضی عمومی 2 (دکتر اعتبار)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+مقدمه ای بر داده کاوی (دکتر خیرخواه)</t>
   </si>
 </sst>
 </file>
@@ -1514,8 +1518,8 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1566,7 +1570,7 @@
     </row>
     <row r="2" spans="1:11" ht="150.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="24" t="s">
@@ -1576,7 +1580,7 @@
       <c r="E2" s="16"/>
       <c r="F2" s="17"/>
       <c r="G2" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="21"/>
       <c r="I2" s="22" t="s">
@@ -1632,14 +1636,14 @@
       <c r="B5" s="2"/>
       <c r="C5" s="9"/>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
-        <v>15</v>
+      <c r="G5" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>33</v>
@@ -1674,7 +1678,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="10"/>
@@ -1682,7 +1686,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>33</v>
@@ -1704,7 +1708,7 @@
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="33" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H8" s="34"/>
       <c r="I8" s="23" t="s">

</xml_diff>

<commit_message>
Added data structure course
</commit_message>
<xml_diff>
--- a/SecondSemester'sSchedule(1402-03).xlsx
+++ b/SecondSemester'sSchedule(1402-03).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniversityAffairs\Management\Schedules\برنامه نیمسال دوم03-1402\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2701A405-0984-4F8E-975E-C00712FF862A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6CA8B6-DA84-4361-84E3-DCDE9D85DDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17323706-087C-48D1-97C3-2A4984637200}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t xml:space="preserve">شنبه
 </t>
@@ -771,6 +771,49 @@
     </r>
   </si>
   <si>
+    <t>مبانی جمعیت شناسی</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">مبانی ترکیبیات
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>کامپایلر (مهندس نجف پور)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+مبانی احتمال
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">مباحثی در علوم کامپیوتر (مهندس فروزش)
+</t>
+    </r>
     <r>
       <rPr>
         <sz val="18"/>
@@ -778,6 +821,91 @@
         <rFont val="B Nazanin"/>
         <charset val="178"/>
       </rPr>
+      <t>اصول طراحی نرم افزار (تئوری، مهندس شاه منصوری)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>مدار منطقی (دکتر خیرخواه)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">مبانی کامپیوتر و برنامه سازی  (دکتر فهیمی)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>مبانی هوش</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFA9E2E"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve"> محاسباتی (دکتر خیرخواه)
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
       <t xml:space="preserve">
 طراحی و تحلیل الگوریتم ها (مهندس شاه منصوری)
 </t>
@@ -785,6 +913,35 @@
     <r>
       <rPr>
         <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>ساختمان داده (خانم مهندس فروزش)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>´</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
         <color rgb="FF7030A0"/>
         <rFont val="B Nazanin"/>
         <charset val="178"/>
@@ -794,68 +951,6 @@
     </r>
   </si>
   <si>
-    <t>مبانی جمعیت شناسی</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">مبانی ترکیبیات
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t>کامپایلر (مهندس نجف پور)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-مبانی احتمال
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">مباحثی در علوم کامپیوتر (مهندس فروزش)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF00B050"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t>اصول طراحی نرم افزار (تئوری، مهندس شاه منصوری)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
     <r>
       <rPr>
         <sz val="18"/>
@@ -863,62 +958,17 @@
         <rFont val="B Nazanin"/>
         <charset val="178"/>
       </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t>مدار منطقی (دکتر خیرخواه)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">مبانی کامپیوتر و برنامه سازی  (دکتر فهیمی)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF00B050"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF00B050"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t>مبانی هوش</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FFFA9E2E"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve"> محاسباتی (دکتر خیرخواه)
-</t>
+      <t>ساختمان داده (خانم مهندس فروزش)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>´</t>
     </r>
   </si>
 </sst>
@@ -926,7 +976,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1005,6 +1055,13 @@
     <font>
       <sz val="18"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Symbol"/>
       <family val="1"/>
       <charset val="2"/>
@@ -1115,7 +1172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1156,16 +1213,55 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1174,59 +1270,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1555,7 +1615,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1599,33 +1659,33 @@
       <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="22"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="150.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="16" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="16"/>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="1:11" ht="110.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -1634,53 +1694,53 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="37"/>
+        <v>47</v>
+      </c>
+      <c r="E3" s="14"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="34" t="s">
+      <c r="A4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="34" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18" t="s">
+      <c r="H4" s="28"/>
+      <c r="I4" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>36</v>
@@ -1688,30 +1748,30 @@
       <c r="H5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" ht="190.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="33" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="23" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="19" t="s">
+      <c r="H6" s="34"/>
+      <c r="I6" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" ht="139.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
@@ -1728,30 +1788,32 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="29" t="s">
+      <c r="A8" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="29" t="s">
+      <c r="F8" s="20"/>
+      <c r="G8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="22"/>
+      <c r="I8" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" ht="145.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -1776,36 +1838,36 @@
       <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="31" t="s">
+      <c r="D10" s="28"/>
+      <c r="E10" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="29" t="s">
+      <c r="F10" s="24"/>
+      <c r="G10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="19" t="s">
+      <c r="H10" s="22"/>
+      <c r="I10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1816,15 +1878,27 @@
         <v>18</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+        <v>48</v>
+      </c>
+      <c r="I11" s="32"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="G2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J2:K11"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
@@ -1840,18 +1914,6 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J2:K11"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="G2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="38" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Added course for statistics group
</commit_message>
<xml_diff>
--- a/SecondSemester'sSchedule(1402-03).xlsx
+++ b/SecondSemester'sSchedule(1402-03).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniversityAffairs\Management\Schedules\برنامه نیمسال دوم03-1402\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DF8349-E2B4-4374-91C3-F9F834D41BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039DDEEC-2E67-493C-8492-794ADD1393DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17323706-087C-48D1-97C3-2A4984637200}"/>
   </bookViews>
@@ -201,10 +201,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">نظریه محاسبه (دکتر خیرخواه)
-</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">
 </t>
@@ -367,51 +363,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t>مبانی کامپیوتر و برنامه سازی (دکتر فهیمی)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF00B050"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t>مبانی آنالیز عددی (دکتر دهقانی)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"> 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">پایگاه داده پیشرفته (مهندس فرشیدی)
 </t>
   </si>
   <si>
@@ -687,22 +639,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">مبانی کامپیوتر و برنامه سازی  (دکتر فهیمی)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF00B050"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="18"/>
         <color rgb="FF00B050"/>
@@ -963,7 +899,104 @@
     </r>
   </si>
   <si>
-    <t>مبانی جمعیت شناسی (دکتر ملتفت)</t>
+    <r>
+      <t xml:space="preserve">نظریه محاسبه (دکتر خیرخواه)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>مبانی کامپیوتر و برنامه سازی (آمار- مهندس شیرعلی)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>مبانی کامپیوتر و برنامه سازی (ریاضی-دکتر فهیمی)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>مبانی آنالیز عددی (دکتر دهقانی)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">مبانی کامپیوتر و برنامه سازی  (ریاضی-دکتر فهیمی)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">پایگاه داده پیشرفته (مهندس فرشیدی)
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">مبانی جمعیت شناسی (دکتر ملتفت)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>مبانی کامپیوتر و برنامه سازی (آمار- مهندس شیرعلی)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1608,8 +1641,8 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1660,24 +1693,24 @@
     </row>
     <row r="2" spans="1:11" ht="150.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="24"/>
       <c r="G2" s="17" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" s="17"/>
     </row>
@@ -1688,7 +1721,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="5"/>
@@ -1700,19 +1733,19 @@
     </row>
     <row r="4" spans="1:11" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="19" t="s">
@@ -1726,19 +1759,19 @@
       <c r="B5" s="2"/>
       <c r="C5" s="9"/>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="17"/>
@@ -1746,11 +1779,11 @@
     </row>
     <row r="6" spans="1:11" ht="190.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" s="35"/>
@@ -1770,7 +1803,7 @@
         <v>51</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="10"/>
@@ -1778,7 +1811,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1788,11 +1821,11 @@
     </row>
     <row r="8" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="15" t="s">
@@ -1800,7 +1833,7 @@
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H8" s="33"/>
       <c r="I8" s="20" t="s">
@@ -1818,13 +1851,13 @@
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>15</v>
@@ -1838,19 +1871,19 @@
     </row>
     <row r="10" spans="1:11" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="26" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F10" s="36"/>
       <c r="G10" s="34" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H10" s="33"/>
       <c r="I10" s="20" t="s">
@@ -1872,7 +1905,7 @@
         <v>18</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="17"/>

</xml_diff>

<commit_message>
Changed Dr. Chachi's course schedule
</commit_message>
<xml_diff>
--- a/SecondSemester'sSchedule(1402-03).xlsx
+++ b/SecondSemester'sSchedule(1402-03).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniversityAffairs\Management\Schedules\برنامه نیمسال دوم03-1402\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039DDEEC-2E67-493C-8492-794ADD1393DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F95207-69D7-4B5C-A8F0-0D04914402D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17323706-087C-48D1-97C3-2A4984637200}"/>
   </bookViews>
@@ -172,21 +172,6 @@
   </si>
   <si>
     <r>
-      <t>مبانی احتمال</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">کامپایلر (مهندس نجف پور)
 </t>
     </r>
@@ -996,6 +981,27 @@
         <charset val="178"/>
       </rPr>
       <t>مبانی کامپیوتر و برنامه سازی (آمار- مهندس شیرعلی)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>مبانی احتمال</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
   </si>
 </sst>
@@ -1199,7 +1205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1219,9 +1225,6 @@
     <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1243,16 +1246,55 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1261,58 +1303,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1642,7 +1645,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1686,234 +1689,246 @@
       <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="25"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="150.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19" t="s">
+      <c r="A2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="28"/>
+      <c r="I2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="17"/>
+      <c r="J2" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="1:11" ht="110.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="14"/>
+        <v>38</v>
+      </c>
+      <c r="E3" s="13"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="38" t="s">
+      <c r="A4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="28"/>
+      <c r="I4" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="9"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
+        <v>24</v>
+      </c>
+      <c r="I5" s="32"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" ht="190.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="26" t="s">
+      <c r="A6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="20" t="s">
+      <c r="H6" s="34"/>
+      <c r="I6" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" ht="139.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>50</v>
       </c>
+      <c r="B7" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="10"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>28</v>
+      <c r="F7" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="15" t="s">
+      <c r="A8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="20" t="s">
+      <c r="F8" s="19"/>
+      <c r="G8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="I8" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" ht="145.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="F9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="35" t="s">
+      <c r="A10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="20" t="s">
+      <c r="H10" s="21"/>
+      <c r="I10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
+      <c r="H11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="32"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="G2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J2:K11"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
@@ -1929,18 +1944,6 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J2:K11"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="G2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="38" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated compiler's time just in Sama
</commit_message>
<xml_diff>
--- a/SecondSemester'sSchedule(1402-03).xlsx
+++ b/SecondSemester'sSchedule(1402-03).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniversityAffairs\Management\Schedules\برنامه نیمسال دوم03-1402\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F95207-69D7-4B5C-A8F0-0D04914402D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59617D7A-5361-4E49-9CDA-51EB9089E988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17323706-087C-48D1-97C3-2A4984637200}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t xml:space="preserve">شنبه
 </t>
@@ -168,21 +168,6 @@
       </rPr>
       <t xml:space="preserve">
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">کامپایلر (مهندس نجف پور)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF00B050"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t>طراحی و تحلیل الگوریتم ها (مهندس شاه منصوری)</t>
     </r>
   </si>
   <si>
@@ -352,10 +337,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">برنامه سازی پیشرفته (تئوری-مهندس شریعتی)
-</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">
 آز سیستم عامل (مهندس شاه منصوری)
@@ -536,31 +517,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">مبانی ترکیبیات
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t>کامپایلر (مهندس نجف پور)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">
 مبانی احتمال
 </t>
@@ -718,68 +674,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-برنامه سازی پیشرفته (تئوری-مهندس شریعتی)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF00B050"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">مقدمه ای بر داده کاوی (دکتر خیرخواه)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF00B050"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="B Nazanin"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">
 </t>
     </r>
@@ -997,6 +891,59 @@
       <rPr>
         <sz val="18"/>
         <color rgb="FF00B050"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">مبانی ترکیبیات
+</t>
+  </si>
+  <si>
+    <t>کامپایلر (مهندس نجف پور)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+برنامه سازی پیشرفته (تئوری-مهندس شریعتی)
+مقدمه ای بر داده کاوی (دکتر خیرخواه)
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF00B050"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>طراحی و تحلیل الگوریتم ها (مهندس شاه منصوری)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">برنامه سازی پیشرفته (تئوری-مهندس شریعتی)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>کامپایلر (مهندس نجف پور)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF7030A0"/>
         <rFont val="B Nazanin"/>
         <charset val="178"/>
       </rPr>
@@ -1246,55 +1193,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1303,19 +1211,58 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1644,8 +1591,8 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1689,33 +1636,35 @@
       <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="30"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11" ht="150.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="31" t="s">
+      <c r="A2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="33"/>
+      <c r="J2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" ht="110.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -1724,89 +1673,89 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="31" t="s">
+      <c r="A4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="8"/>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
+        <v>23</v>
+      </c>
+      <c r="I5" s="19"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:11" ht="190.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="27" t="s">
+      <c r="A6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="34"/>
-      <c r="I6" s="32" t="s">
+      <c r="H6" s="25"/>
+      <c r="I6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:11" ht="139.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="9"/>
@@ -1814,53 +1763,53 @@
         <v>16</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="18" t="s">
+      <c r="A8" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="32" t="s">
+      <c r="F8" s="15"/>
+      <c r="G8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="31"/>
+      <c r="I8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:11" ht="145.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F9" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>15</v>
@@ -1868,36 +1817,36 @@
       <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="32"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:11" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="23" t="s">
+      <c r="A10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="32" t="s">
+      <c r="D10" s="17"/>
+      <c r="E10" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="34"/>
+      <c r="G10" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="31"/>
+      <c r="I10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1908,27 +1857,15 @@
         <v>18</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="32"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
+        <v>44</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="G2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J2:K11"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
@@ -1944,6 +1881,18 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J2:K11"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="G2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="38" orientation="landscape" r:id="rId1"/>

</xml_diff>